<commit_message>
add extra files + cmd
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,6 +434,11 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>sex</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>timestamp</t>
         </is>
       </c>
@@ -451,7 +456,298 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2026-01-03T11:02:58</t>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2026-01-03T11:38:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2026-01-04</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Samantha Gracia</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2026-01-03T11:41:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2026-01-03</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Shiro Budiman</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2026-01-03T11:41:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2026-01-04</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Ricky Adikurnia</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2026-01-03T14:15:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2026-01-04</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Siat Cynthia</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2026-01-03T14:15:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2026-01-03</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Leonardo Kwan</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2026-01-03T14:23:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2026-01-03</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Darren Nathanael Budiman</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2026-01-03T14:23:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2026-01-03</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Wilson Thiesman</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2026-01-03T19:40:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2026-01-03</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Haydee Judith Manuella</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2026-01-03T19:40:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2026-01-03</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Darren Nathanael Budiman</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2026-01-03T19:40:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2026-01-03</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Marcello Pardede</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2026-01-03T19:50:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2026-01-04</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Darren Nathanael Budiman</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2026-01-03T19:52:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2026-01-04</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Leonardo Kwan</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2026-01-03T19:52:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2026-01-03</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Richard</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2026-01-03T19:52:50</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add attendance recorded feature
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -15,7 +15,7 @@
   </definedNames>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
   <pivotCaches>
-    <pivotCache cacheId="34" r:id="rId4"/>
+    <pivotCache cacheId="7" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -133,20 +133,22 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" refreshedBy="Darren N. Budiman" refreshedDate="46033.59092118056" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="27" r:id="rId1">
+<pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" refreshedBy="Darren N. Budiman" refreshedDate="46047.56249467593" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="76" r:id="rId1">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:D1048576" sheet="Attendance"/>
   </cacheSource>
   <cacheFields count="4">
     <cacheField name="event_date" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
-      <sharedItems count="3" containsBlank="1">
+      <sharedItems count="5" containsBlank="1">
         <s v="2026-01-11"/>
+        <s v="2026-01-18"/>
+        <s v="2026-01-25"/>
         <m/>
         <s v="2026-01-10" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="full_name" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
-      <sharedItems count="29" containsBlank="1">
+      <sharedItems count="49" containsBlank="1">
         <s v="Timothy Robby"/>
         <s v="David Tjoe (Mu Shi)"/>
         <s v="Ricky Adikurnia"/>
@@ -173,9 +175,29 @@
         <s v="STEPHANIE KOWINTO"/>
         <s v="Wilson Thiesman"/>
         <s v="Richard Valent Tanuwijaya"/>
+        <s v="Felicia Wijaya"/>
+        <s v="Michael Himawan"/>
+        <s v="Felicia Widjaja"/>
+        <s v="Marvin Ali"/>
+        <s v="Nicholas Bungaran Martua"/>
+        <s v="Lingga Ekaputra Lucky Suryajaya"/>
+        <s v="Grace Regina Layndra"/>
+        <s v="Jocelyn Meilina Woenardi"/>
+        <s v="Axell Nathaniel Wahyu Sagala"/>
+        <s v="Sheryl Jovaha Sianipar"/>
+        <s v="Leonardo Kwan"/>
+        <s v="Vailyn"/>
+        <s v="Hanna Jane"/>
+        <s v="Carla Edlyn"/>
+        <s v="William Jefferson"/>
+        <s v="Dave Sinaga"/>
+        <s v="Wilson Orlando"/>
+        <s v="Marcello Raphael Pardede"/>
+        <s v="Kentzo Pietro"/>
+        <s v="Clarence Victorio Widiyanto"/>
+        <s v="Vincent Aurelius Johannes"/>
         <m/>
         <s v="Magnus Hosea" u="1"/>
-        <s v="Carla Edlyn" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="sex" uniqueList="1" numFmtId="0" sqlType="0" hierarchy="0" level="0" databaseField="1">
@@ -193,7 +215,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -351,8 +373,302 @@
     <s v="2026-01-11T14:08:47"/>
   </r>
   <r>
-    <x v="1"/>
+    <x v="0"/>
     <x v="26"/>
+    <x v="1"/>
+    <s v="2026-01-11T14:11:54"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="27"/>
+    <x v="0"/>
+    <s v="2026-01-11T14:12:05"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="28"/>
+    <x v="1"/>
+    <s v="2026-01-11T14:16:57"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="29"/>
+    <x v="0"/>
+    <s v="2026-01-11T14:17:03"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="30"/>
+    <x v="0"/>
+    <s v="2026-01-11T14:20:34"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="31"/>
+    <x v="0"/>
+    <s v="2026-01-11T14:40:47"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="32"/>
+    <x v="1"/>
+    <s v="2026-01-11T14:41:12"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="33"/>
+    <x v="1"/>
+    <s v="2026-01-18T13:21:49"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="10"/>
+    <x v="0"/>
+    <s v="2026-01-18T13:21:49"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="11"/>
+    <x v="1"/>
+    <s v="2026-01-18T13:21:49"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="34"/>
+    <x v="0"/>
+    <s v="2026-01-18T13:29:41"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="25"/>
+    <x v="0"/>
+    <s v="2026-01-18T13:29:50"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="0"/>
+    <s v="2026-01-18T13:29:56"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="9"/>
+    <x v="0"/>
+    <s v="2026-01-18T13:30:01"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="35"/>
+    <x v="1"/>
+    <s v="2026-01-18T13:30:09"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="0"/>
+    <s v="2026-01-18T13:30:21"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="1"/>
+    <s v="2026-01-18T13:30:29"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="2026-01-18T13:30:42"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="0"/>
+    <s v="2026-01-18T13:39:14"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="2026-01-18T13:39:45"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="36"/>
+    <x v="0"/>
+    <s v="2026-01-18T13:41:05"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="17"/>
+    <x v="1"/>
+    <s v="2026-01-18T13:50:09"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="8"/>
+    <x v="1"/>
+    <s v="2026-01-18T13:50:13"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="32"/>
+    <x v="1"/>
+    <s v="2026-01-18T14:00:19"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="37"/>
+    <x v="1"/>
+    <s v="2026-01-18T14:01:56"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="15"/>
+    <x v="0"/>
+    <s v="2026-01-18T14:02:06"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="38"/>
+    <x v="1"/>
+    <s v="2026-01-18T14:04:36"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="39"/>
+    <x v="1"/>
+    <s v="2026-01-18T14:04:42"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="14"/>
+    <x v="1"/>
+    <s v="2026-01-18T14:04:55"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="30"/>
+    <x v="0"/>
+    <s v="2026-01-18T14:05:55"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="16"/>
+    <x v="0"/>
+    <s v="2026-01-18T14:06:18"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="40"/>
+    <x v="0"/>
+    <s v="2026-01-18T14:06:37"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="18"/>
+    <x v="1"/>
+    <s v="2026-01-18T14:15:05"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="41"/>
+    <x v="0"/>
+    <s v="2026-01-18T14:29:50"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="42"/>
+    <x v="0"/>
+    <s v="2026-01-18T14:30:02"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="43"/>
+    <x v="0"/>
+    <s v="2026-01-18T14:33:31"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="19"/>
+    <x v="0"/>
+    <s v="2026-01-18T16:05:29"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="44"/>
+    <x v="0"/>
+    <s v="2026-01-18T16:05:45"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="45"/>
+    <x v="0"/>
+    <s v="2026-01-18T16:09:48"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="46"/>
+    <x v="0"/>
+    <s v="2026-01-25T13:29:38"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="33"/>
+    <x v="1"/>
+    <s v="2026-01-25T13:29:38"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="30"/>
+    <x v="0"/>
+    <s v="2026-01-25T13:29:38"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="18"/>
+    <x v="1"/>
+    <s v="2026-01-25T13:29:38"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="36"/>
+    <x v="0"/>
+    <s v="2026-01-25T13:29:38"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="24"/>
+    <x v="0"/>
+    <s v="2026-01-25T13:29:38"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="10"/>
+    <x v="0"/>
+    <s v="2026-01-25T13:29:38"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="11"/>
+    <x v="1"/>
+    <s v="2026-01-25T13:29:38"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="38"/>
+    <x v="1"/>
+    <s v="2026-01-25T13:29:38"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="8"/>
+    <x v="1"/>
+    <s v="2026-01-25T13:29:38"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <x v="47"/>
     <x v="2"/>
     <m/>
   </r>
@@ -360,26 +676,28 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="34" dataOnRows="0" dataCaption="Values" showError="0" showMissing="1" updatedVersion="8" minRefreshableVersion="3" asteriskTotals="0" showItems="1" editData="0" disableFieldList="0" showCalcMbrs="1" visualTotals="1" showMultipleLabel="1" showDataDropDown="1" showDrill="1" printDrill="0" showMemberPropertyTips="1" showDataTips="1" enableWizard="1" enableDrill="1" enableFieldProperties="1" preserveFormatting="1" useAutoFormatting="1" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" rowGrandTotals="1" colGrandTotals="1" fieldPrintTitles="0" itemPrintTitles="1" mergeItem="0" showDropZones="1" createdVersion="8" indent="0" showEmptyRow="0" showEmptyCol="0" showHeaders="1" compact="0" outline="0" outlineData="0" compactData="0" published="0" gridDropZones="0" immersive="1" multipleFieldFilters="0" chartFormat="0" fieldListSortAscending="0" mdxSubqueries="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" r:id="rId1">
-  <location ref="A3:C32" firstHeaderRow="1" firstDataRow="1" firstDataCol="2" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="7" dataOnRows="0" dataCaption="Values" showError="0" showMissing="1" updatedVersion="8" minRefreshableVersion="3" asteriskTotals="0" showItems="1" editData="0" disableFieldList="0" showCalcMbrs="1" visualTotals="1" showMultipleLabel="1" showDataDropDown="1" showDrill="1" printDrill="0" showMemberPropertyTips="1" showDataTips="1" enableWizard="1" enableDrill="1" enableFieldProperties="1" preserveFormatting="1" useAutoFormatting="1" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" rowGrandTotals="1" colGrandTotals="1" fieldPrintTitles="0" itemPrintTitles="1" mergeItem="0" showDropZones="1" createdVersion="8" indent="0" showEmptyRow="0" showEmptyCol="0" showHeaders="1" compact="0" outline="0" outlineData="0" compactData="0" published="0" gridDropZones="0" immersive="1" multipleFieldFilters="0" chartFormat="0" fieldListSortAscending="0" mdxSubqueries="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" r:id="rId1">
+  <location ref="A3:C16" firstHeaderRow="1" firstDataRow="1" firstDataCol="2" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="4">
     <pivotField axis="axisPage" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" multipleItemSelectionAllowed="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1">
-      <items count="4">
-        <item t="data" h="1" sd="1" m="1" x="2"/>
+      <items count="6">
+        <item t="data" h="1" sd="1" m="1" x="4"/>
+        <item t="data" h="1" sd="1" x="3"/>
+        <item t="data" h="1" sd="1" x="0"/>
         <item t="data" h="1" sd="1" x="1"/>
-        <item t="data" sd="1" x="0"/>
+        <item t="data" sd="1" x="2"/>
         <item t="default" sd="1"/>
       </items>
     </pivotField>
     <pivotField axis="axisRow" dataField="1" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1">
-      <items count="30">
+      <items count="50">
         <item t="data" sd="1" x="10"/>
         <item t="data" sd="1" x="11"/>
-        <item t="data" sd="1" x="26"/>
-        <item t="data" sd="1" m="1" x="27"/>
+        <item t="data" sd="1" x="47"/>
+        <item t="data" sd="1" m="1" x="48"/>
         <item t="data" sd="1" x="1"/>
         <item t="data" sd="1" x="4"/>
-        <item t="data" sd="1" m="1" x="28"/>
+        <item t="data" sd="1" x="39"/>
         <item t="data" sd="1" x="8"/>
         <item t="data" sd="1" x="6"/>
         <item t="data" sd="1" x="2"/>
@@ -402,6 +720,26 @@
         <item t="data" sd="1" x="23"/>
         <item t="data" sd="1" x="24"/>
         <item t="data" sd="1" x="25"/>
+        <item t="data" sd="1" x="26"/>
+        <item t="data" sd="1" x="27"/>
+        <item t="data" sd="1" x="28"/>
+        <item t="data" sd="1" x="29"/>
+        <item t="data" sd="1" x="30"/>
+        <item t="data" sd="1" x="31"/>
+        <item t="data" sd="1" x="32"/>
+        <item t="data" sd="1" x="33"/>
+        <item t="data" sd="1" x="34"/>
+        <item t="data" sd="1" x="35"/>
+        <item t="data" sd="1" x="36"/>
+        <item t="data" sd="1" x="37"/>
+        <item t="data" sd="1" x="38"/>
+        <item t="data" sd="1" x="40"/>
+        <item t="data" sd="1" x="41"/>
+        <item t="data" sd="1" x="42"/>
+        <item t="data" sd="1" x="43"/>
+        <item t="data" sd="1" x="44"/>
+        <item t="data" sd="1" x="45"/>
+        <item t="data" sd="1" x="46"/>
         <item t="default" sd="1"/>
       </items>
     </pivotField>
@@ -419,37 +757,22 @@
     <field x="2"/>
     <field x="1"/>
   </rowFields>
-  <rowItems count="29">
+  <rowItems count="13">
     <i t="data" r="0" i="0">
       <x v="0"/>
       <x v="1"/>
     </i>
     <i t="data" r="1" i="0">
-      <x v="5"/>
-    </i>
-    <i t="data" r="1" i="0">
       <x v="7"/>
-    </i>
-    <i t="data" r="1" i="0">
-      <x v="12"/>
-    </i>
-    <i t="data" r="1" i="0">
-      <x v="15"/>
-    </i>
-    <i t="data" r="1" i="0">
-      <x v="17"/>
-    </i>
-    <i t="data" r="1" i="0">
-      <x v="20"/>
     </i>
     <i t="data" r="1" i="0">
       <x v="21"/>
     </i>
     <i t="data" r="1" i="0">
-      <x v="23"/>
+      <x v="36"/>
     </i>
     <i t="data" r="1" i="0">
-      <x v="26"/>
+      <x v="41"/>
     </i>
     <i t="default" r="0" i="0">
       <x v="0"/>
@@ -459,49 +782,16 @@
       <x v="0"/>
     </i>
     <i t="data" r="1" i="0">
-      <x v="4"/>
-    </i>
-    <i t="data" r="1" i="0">
-      <x v="8"/>
-    </i>
-    <i t="data" r="1" i="0">
-      <x v="9"/>
-    </i>
-    <i t="data" r="1" i="0">
-      <x v="10"/>
-    </i>
-    <i t="data" r="1" i="0">
-      <x v="11"/>
-    </i>
-    <i t="data" r="1" i="0">
-      <x v="13"/>
-    </i>
-    <i t="data" r="1" i="0">
-      <x v="14"/>
-    </i>
-    <i t="data" r="1" i="0">
-      <x v="16"/>
-    </i>
-    <i t="data" r="1" i="0">
-      <x v="18"/>
-    </i>
-    <i t="data" r="1" i="0">
-      <x v="19"/>
-    </i>
-    <i t="data" r="1" i="0">
-      <x v="22"/>
-    </i>
-    <i t="data" r="1" i="0">
-      <x v="24"/>
-    </i>
-    <i t="data" r="1" i="0">
-      <x v="25"/>
-    </i>
-    <i t="data" r="1" i="0">
       <x v="27"/>
     </i>
     <i t="data" r="1" i="0">
-      <x v="28"/>
+      <x v="33"/>
+    </i>
+    <i t="data" r="1" i="0">
+      <x v="39"/>
+    </i>
+    <i t="data" r="1" i="0">
+      <x v="48"/>
     </i>
     <i t="default" r="0" i="0">
       <x v="1"/>
@@ -812,10 +1102,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B76" sqref="B68:B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1574,6 +1864,930 @@
         </is>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Jocelyn Meilina Woenardi</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>2026-01-18T13:21:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Darren Nathanael Budiman</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>2026-01-18T13:21:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Haydee Judith Manuella</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>2026-01-18T13:21:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Axell Nathaniel Wahyu Sagala</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>2026-01-18T13:29:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Richard Valent Tanuwijaya</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>2026-01-18T13:29:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Wilson Chistopher Husein</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>2026-01-18T13:29:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Felix Wijaya</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>2026-01-18T13:30:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Sheryl Jovaha Sianipar</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>2026-01-18T13:30:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Mikael Alden Nurjadi</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>2026-01-18T13:30:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Neria Yesika Sugiyanto</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>2026-01-18T13:30:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>David Tjoe (Mu Shi)</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>2026-01-18T13:30:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Magnus Hosea Rangen Jaya</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>2026-01-18T13:39:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Timothy Robby</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>2026-01-18T13:39:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Leonardo Kwan</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>2026-01-18T13:41:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Lissye Lau</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>2026-01-18T13:50:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Siat Cynthia</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>2026-01-18T13:50:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Grace Regina Layndra</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>2026-01-18T14:00:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Vailyn</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>2026-01-18T14:01:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Christopher Noel Suherman</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>2026-01-18T14:02:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Hanna Jane</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>2026-01-18T14:04:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Carla Edlyn</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>2026-01-18T14:04:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Jennifer Kurniawan</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>2026-01-18T14:04:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Nicholas Bungaran Martua</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>2026-01-18T14:05:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Nathan Setyo</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>2026-01-18T14:06:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>William Jefferson</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>2026-01-18T14:06:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Caroline Avery Tanto</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>2026-01-18T14:15:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Dave Sinaga</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>2026-01-18T14:29:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Wilson Orlando</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>2026-01-18T14:30:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Marcello Raphael Pardede</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>2026-01-18T14:33:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Joshua Viencent Tandibrata</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>2026-01-18T16:05:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Kentzo Pietro</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>2026-01-18T16:05:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2026-01-18</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Clarence Victorio Widiyanto</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>2026-01-18T16:09:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Vincent Aurelius Johannes</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>2026-01-25T13:29:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Jocelyn Meilina Woenardi</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>2026-01-25T13:29:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Nicholas Bungaran Martua</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>2026-01-25T13:29:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Caroline Avery Tanto</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>2026-01-25T13:29:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Leonardo Kwan</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>2026-01-25T13:29:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Wilson Thiesman</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>2026-01-25T13:29:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Darren Nathanael Budiman</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>2026-01-25T13:29:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Haydee Judith Manuella</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>2026-01-25T13:29:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Hanna Jane</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>2026-01-25T13:29:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2026-01-25</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Siat Cynthia</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>2026-01-25T13:29:38</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1585,10 +2799,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B89"/>
+  <dimension ref="A1:B93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2661,6 +3875,54 @@
       <c r="B89" t="inlineStr">
         <is>
           <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Vailyn</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>F</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>William Jefferson</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Kentzo Pietro</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Clarence Victorio Widiyanto</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>M</t>
         </is>
       </c>
     </row>
@@ -2680,16 +3942,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col width="25.5" bestFit="1" customWidth="1" style="2" min="1" max="1"/>
-    <col width="22.33203125" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
+    <col width="21.83203125" bestFit="1" customWidth="1" style="2" min="2" max="2"/>
     <col width="15.6640625" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
   </cols>
   <sheetData>
@@ -2701,7 +3963,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>2026-01-11</t>
+          <t>2026-01-25</t>
         </is>
       </c>
     </row>
@@ -2740,7 +4002,7 @@
     <row r="5">
       <c r="B5" t="inlineStr">
         <is>
-          <t>Dorothy Andriani Setyawan</t>
+          <t>Siat Cynthia</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -2750,7 +4012,7 @@
     <row r="6">
       <c r="B6" t="inlineStr">
         <is>
-          <t>Siat Cynthia</t>
+          <t>Caroline Avery Tanto</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -2760,7 +4022,7 @@
     <row r="7">
       <c r="B7" t="inlineStr">
         <is>
-          <t>Neria Yesika Sugiyanto</t>
+          <t>Jocelyn Meilina Woenardi</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -2770,7 +4032,7 @@
     <row r="8">
       <c r="B8" t="inlineStr">
         <is>
-          <t>Betty Lee</t>
+          <t>Hanna Jane</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -2778,19 +4040,24 @@
       </c>
     </row>
     <row r="9">
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Jennifer Kurniawan</t>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>F Total</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Lissye Lau</t>
+          <t>Darren Nathanael Budiman</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -2800,7 +4067,7 @@
     <row r="11">
       <c r="B11" t="inlineStr">
         <is>
-          <t>Caroline Avery Tanto</t>
+          <t>Wilson Thiesman</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -2810,7 +4077,7 @@
     <row r="12">
       <c r="B12" t="inlineStr">
         <is>
-          <t>Awen Caroline</t>
+          <t>Nicholas Bungaran Martua</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -2820,7 +4087,7 @@
     <row r="13">
       <c r="B13" t="inlineStr">
         <is>
-          <t>STEPHANIE KOWINTO</t>
+          <t>Leonardo Kwan</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -2828,198 +4095,33 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>F Total</t>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Vincent Aurelius Johannes</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Darren Nathanael Budiman</t>
+          <t>M Total</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>David Tjoe (Mu Shi)</t>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Grand Total</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Wilson Chistopher Husein</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Ricky Adikurnia</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Timothy Robby</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Magnus Hosea Rangen Jaya</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Mikael Alden Nurjadi</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Felix Wijaya</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Tsang Robby</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Christopher Noel Suherman</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Nathan Setyo</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Joshua Viencent Tandibrata</t>
-        </is>
-      </c>
-      <c r="C26" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Ferris Prima Nugraha</t>
-        </is>
-      </c>
-      <c r="C27" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>WILFRID AZARIAH</t>
-        </is>
-      </c>
-      <c r="C28" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Wilson Thiesman</t>
-        </is>
-      </c>
-      <c r="C29" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Richard Valent Tanuwijaya</t>
-        </is>
-      </c>
-      <c r="C30" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>M Total</t>
-        </is>
-      </c>
-      <c r="C31" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Grand Total</t>
-        </is>
-      </c>
-      <c r="C32" t="n">
-        <v>26</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>